<commit_message>
All the comments for now
</commit_message>
<xml_diff>
--- a/zzyTest/Goods.xlsx
+++ b/zzyTest/Goods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\isem2006\ISEM_Grop_proj\zzyTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LYLJack\Desktop\isemGroupProject\Version2\ISEM_Grop_proj-master\ISEM_Grop_proj\zzyTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15451BEF-9B1A-4D83-A1AA-0F4FFACBE41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FF07A6-DA73-4D78-8E99-E4AE1C5315EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="16044" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -495,17 +495,17 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.25" customWidth="1"/>
-    <col min="2" max="2" width="17.08203125" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -519,7 +519,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -533,7 +533,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -547,7 +547,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -561,7 +561,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -575,7 +575,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -589,7 +589,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -603,7 +603,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -617,7 +617,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -631,7 +631,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -645,7 +645,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -659,7 +659,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -673,7 +673,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -687,7 +687,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -701,7 +701,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -715,7 +715,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -729,7 +729,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -743,7 +743,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -757,7 +757,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -771,7 +771,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -785,7 +785,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>

</xml_diff>